<commit_message>
Added more history files
</commit_message>
<xml_diff>
--- a/accuracies_compared.xlsx
+++ b/accuracies_compared.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/philippmetzger/Documents/GitHub/Deep_Learning_Project_Group_10/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{27462465-D068-4643-B2E2-97860D20A512}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E034A365-70C2-694A-80E8-EF6E561592D6}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="accuracies_compared" sheetId="1" r:id="rId1"/>
@@ -20,19 +20,25 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>val_acc_base</t>
   </si>
   <si>
     <t>val_acc_dropout_1</t>
   </si>
+  <si>
+    <t>val_acc_augmented_1_shuffle_false</t>
+  </si>
+  <si>
+    <t>val_acc_augmented_1_shuffle_true</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -163,6 +169,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -509,8 +522,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -624,7 +638,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>accuracies_compared!$E$1</c:f>
+              <c:f>accuracies_compared!$B$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -647,7 +661,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>accuracies_compared!$E$2:$E$31</c:f>
+              <c:f>accuracies_compared!$B$5:$B$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -747,7 +761,7 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-D7D8-C042-A622-1013D326515F}"/>
+              <c16:uniqueId val="{00000000-0249-C14F-8922-9E59B2E57466}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -756,7 +770,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>accuracies_compared!$F$1</c:f>
+              <c:f>accuracies_compared!$C$4</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -779,7 +793,7 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>accuracies_compared!$F$2:$F$31</c:f>
+              <c:f>accuracies_compared!$C$5:$C$34</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="30"/>
@@ -879,7 +893,271 @@
           <c:smooth val="0"/>
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000001-D7D8-C042-A622-1013D326515F}"/>
+              <c16:uniqueId val="{00000001-0249-C14F-8922-9E59B2E57466}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>accuracies_compared!$D$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>val_acc_augmented_1_shuffle_false</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent3"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>accuracies_compared!$D$5:$D$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.115</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26300000000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.26600000000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.312</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.32700000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41399999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.40100000000000002</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.442</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.42899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.47599999999999998</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.42699999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46200000000000002</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.45600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.46</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.435</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.45600000000000002</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.48799999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.45400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.497</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.46600000000000003</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.46700000000000003</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.50900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.47499999999999998</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.503</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.498</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.53400000000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-0249-C14F-8922-9E59B2E57466}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>accuracies_compared!$E$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>val_acc_augmented_1_shuffle_true</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent4"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>accuracies_compared!$E$5:$E$34</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="30"/>
+                <c:pt idx="0">
+                  <c:v>0.21099999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.20100001000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.26300001000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.29699998999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.375</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.36899999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41800000999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.41299998999999998</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.41600000999999998</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.43200000999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.46300000000000002</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.46399998999999997</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.47499998999999998</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.44900000000000001</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.45100001000000001</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.47499998999999998</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.40000001000000002</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.45400000000000001</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.45899999000000002</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.45100001000000001</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.46900001000000002</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.46700001000000002</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.48599999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.44800001</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.45800000000000002</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.47099998999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-0249-C14F-8922-9E59B2E57466}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -892,11 +1170,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="94669535"/>
-        <c:axId val="94545791"/>
+        <c:axId val="276746815"/>
+        <c:axId val="276748463"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="94669535"/>
+        <c:axId val="276746815"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -938,7 +1216,7 @@
             <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94545791"/>
+        <c:crossAx val="276748463"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -946,7 +1224,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="94545791"/>
+        <c:axId val="276748463"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -997,7 +1275,7 @@
             <a:endParaRPr lang="en-DE"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="94669535"/>
+        <c:crossAx val="276746815"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1644,23 +1922,23 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>692150</xdr:colOff>
-      <xdr:row>6</xdr:row>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>196850</xdr:colOff>
+      <xdr:row>4</xdr:row>
       <xdr:rowOff>50800</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>355600</xdr:colOff>
-      <xdr:row>25</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>508000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>25400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1">
+        <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D0DE45A3-BC4D-5744-9D17-2EE9D27D6C0A}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{15AB6D0A-492B-A541-B435-4146E43AB90A}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1977,351 +2255,542 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F31"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A4:E34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L30" sqref="L30"/>
+      <selection activeCell="J33" sqref="J33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="E1" t="s">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" t="s">
+      <c r="C4" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2">
+      <c r="D4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5">
         <v>0</v>
       </c>
-      <c r="E2">
+      <c r="B5">
         <v>0.19499999300000001</v>
       </c>
-      <c r="F2">
+      <c r="C5">
         <v>0.23800001000000001</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3">
+      <c r="D5" s="1">
+        <v>0.115</v>
+      </c>
+      <c r="E5">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6">
         <v>1</v>
       </c>
-      <c r="E3">
+      <c r="B6">
         <v>0.187999994</v>
       </c>
-      <c r="F3">
+      <c r="C6">
         <v>0.33300000000000002</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4">
+      <c r="D6" s="1">
+        <v>0.24</v>
+      </c>
+      <c r="E6">
+        <v>0.20100001000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7">
         <v>2</v>
       </c>
-      <c r="E4">
+      <c r="B7">
         <v>0.29899999500000002</v>
       </c>
-      <c r="F4">
+      <c r="C7">
         <v>0.35699998999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5">
+      <c r="D7" s="1">
+        <v>0.26300000000000001</v>
+      </c>
+      <c r="E7">
+        <v>0.26300001000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8">
         <v>3</v>
       </c>
-      <c r="E5">
+      <c r="B8">
         <v>0.335999995</v>
       </c>
-      <c r="F5">
+      <c r="C8">
         <v>0.38699999000000002</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6">
+      <c r="D8" s="1">
+        <v>0.29799999999999999</v>
+      </c>
+      <c r="E8">
+        <v>0.29699998999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9">
         <v>4</v>
       </c>
-      <c r="E6">
+      <c r="B9">
         <v>0.37799999099999998</v>
       </c>
-      <c r="F6">
+      <c r="C9">
         <v>0.435</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7">
+      <c r="D9" s="1">
+        <v>0.26600000000000001</v>
+      </c>
+      <c r="E9">
+        <v>0.375</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10">
         <v>5</v>
       </c>
-      <c r="E7">
+      <c r="B10">
         <v>0.439999998</v>
       </c>
-      <c r="F7">
+      <c r="C10">
         <v>0.43399999</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8">
+      <c r="D10" s="1">
+        <v>0.312</v>
+      </c>
+      <c r="E10">
+        <v>0.36899999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11">
         <v>6</v>
       </c>
-      <c r="E8">
+      <c r="B11">
         <v>0.547999978</v>
       </c>
-      <c r="F8">
+      <c r="C11">
         <v>0.47099998999999998</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9">
+      <c r="D11" s="1">
+        <v>0.32700000000000001</v>
+      </c>
+      <c r="E11">
+        <v>0.38400000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
         <v>7</v>
       </c>
-      <c r="E9">
+      <c r="B12">
         <v>0.46500000400000002</v>
       </c>
-      <c r="F9">
+      <c r="C12">
         <v>0.50900000000000001</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10">
+      <c r="D12" s="1">
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="E12">
+        <v>0.37</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13">
         <v>8</v>
       </c>
-      <c r="E10">
+      <c r="B13">
         <v>0.52300000199999996</v>
       </c>
-      <c r="F10">
+      <c r="C13">
         <v>0.50700003000000005</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A11">
+      <c r="D13" s="1">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="E13">
+        <v>0.41800000999999998</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14">
         <v>9</v>
       </c>
-      <c r="E11">
+      <c r="B14">
         <v>0.50300002099999996</v>
       </c>
-      <c r="F11">
+      <c r="C14">
         <v>0.51999998000000003</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12">
+      <c r="D14" s="1">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="E14">
+        <v>0.41299998999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15">
         <v>10</v>
       </c>
-      <c r="E12">
+      <c r="B15">
         <v>0.48500001399999998</v>
       </c>
-      <c r="F12">
+      <c r="C15">
         <v>0.56400001</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A13">
+      <c r="D15" s="1">
+        <v>0.442</v>
+      </c>
+      <c r="E15">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
         <v>11</v>
       </c>
-      <c r="E13">
+      <c r="B16">
         <v>0.47999998900000002</v>
       </c>
-      <c r="F13">
+      <c r="C16">
         <v>0.50199996999999996</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A14">
+      <c r="D16" s="1">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="E16">
+        <v>0.41600000999999998</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17">
         <v>12</v>
       </c>
-      <c r="E14">
+      <c r="B17">
         <v>0.54299998299999996</v>
       </c>
-      <c r="F14">
+      <c r="C17">
         <v>0.53200000999999997</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A15">
+      <c r="D17" s="1">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="E17">
+        <v>0.43200000999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18">
         <v>13</v>
       </c>
-      <c r="E15">
+      <c r="B18">
         <v>0.541000009</v>
       </c>
-      <c r="F15">
+      <c r="C18">
         <v>0.55500000999999999</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A16">
+      <c r="D18" s="1">
+        <v>0.42699999999999999</v>
+      </c>
+      <c r="E18">
+        <v>0.46300000000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19">
         <v>14</v>
       </c>
-      <c r="E16">
+      <c r="B19">
         <v>0.573000014</v>
       </c>
-      <c r="F16">
+      <c r="C19">
         <v>0.56999999000000001</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A17">
+      <c r="D19" s="1">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="E19">
+        <v>0.46399998999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20">
         <v>15</v>
       </c>
-      <c r="E17">
+      <c r="B20">
         <v>0.53799998800000004</v>
       </c>
-      <c r="F17">
+      <c r="C20">
         <v>0.57399999999999995</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A18">
+      <c r="D20" s="1">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="E20">
+        <v>0.44</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21">
         <v>16</v>
       </c>
-      <c r="E18">
+      <c r="B21">
         <v>0.57800000900000004</v>
       </c>
-      <c r="F18">
+      <c r="C21">
         <v>0.56999999000000001</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A19">
+      <c r="D21" s="1">
+        <v>0.46</v>
+      </c>
+      <c r="E21">
+        <v>0.47499998999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22">
         <v>17</v>
       </c>
-      <c r="E19">
+      <c r="B22">
         <v>0.56999999300000004</v>
       </c>
-      <c r="F19">
+      <c r="C22">
         <v>0.60000001999999997</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A20">
+      <c r="D22" s="1">
+        <v>0.435</v>
+      </c>
+      <c r="E22">
+        <v>0.44900000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23">
         <v>18</v>
       </c>
-      <c r="E20">
+      <c r="B23">
         <v>0.545000017</v>
       </c>
-      <c r="F20">
+      <c r="C23">
         <v>0.58200001999999995</v>
       </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A21">
+      <c r="D23" s="1">
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="E23">
+        <v>0.45100001000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24">
         <v>19</v>
       </c>
-      <c r="E21">
+      <c r="B24">
         <v>0.47900000199999998</v>
       </c>
-      <c r="F21">
+      <c r="C24">
         <v>0.58299999999999996</v>
       </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A22">
+      <c r="D24" s="1">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="E24">
+        <v>0.47499998999999998</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25">
         <v>20</v>
       </c>
-      <c r="E22">
+      <c r="B25">
         <v>0.527999997</v>
       </c>
-      <c r="F22">
+      <c r="C25">
         <v>0.57300001</v>
       </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A23">
+      <c r="D25" s="1">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.40000001000000002</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
         <v>21</v>
       </c>
-      <c r="E23">
+      <c r="B26">
         <v>0.55900001499999996</v>
       </c>
-      <c r="F23">
+      <c r="C26">
         <v>0.59699999999999998</v>
       </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A24">
+      <c r="D26" s="1">
+        <v>0.497</v>
+      </c>
+      <c r="E26">
+        <v>0.45400000000000001</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27">
         <v>22</v>
       </c>
-      <c r="E24">
+      <c r="B27">
         <v>0.52499997600000003</v>
       </c>
-      <c r="F24">
+      <c r="C27">
         <v>0.63</v>
       </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A25">
+      <c r="D27" s="1">
+        <v>0.46600000000000003</v>
+      </c>
+      <c r="E27">
+        <v>0.45899999000000002</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28">
         <v>23</v>
       </c>
-      <c r="E25">
+      <c r="B28">
         <v>0.555999994</v>
       </c>
-      <c r="F25">
+      <c r="C28">
         <v>0.61699998</v>
       </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26">
+      <c r="D28" s="1">
+        <v>0.46700000000000003</v>
+      </c>
+      <c r="E28">
+        <v>0.45100001000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
         <v>24</v>
       </c>
-      <c r="E26">
+      <c r="B29">
         <v>0.53500002599999996</v>
       </c>
-      <c r="F26">
+      <c r="C29">
         <v>0.61900001999999998</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A27">
+      <c r="D29" s="1">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="E29">
+        <v>0.46900001000000002</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30">
         <v>25</v>
       </c>
-      <c r="E27">
+      <c r="B30">
         <v>0.569000006</v>
       </c>
-      <c r="F27">
+      <c r="C30">
         <v>0.60600001000000003</v>
       </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A28">
+      <c r="D30" s="1">
+        <v>0.47499999999999998</v>
+      </c>
+      <c r="E30">
+        <v>0.46700001000000002</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31">
         <v>26</v>
       </c>
-      <c r="E28">
+      <c r="B31">
         <v>0.56099999</v>
       </c>
-      <c r="F28">
+      <c r="C31">
         <v>0.59399997999999998</v>
       </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29">
+      <c r="D31" s="1">
+        <v>0.503</v>
+      </c>
+      <c r="E31">
+        <v>0.48599999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32">
         <v>27</v>
       </c>
-      <c r="E29">
+      <c r="B32">
         <v>0.54699999099999996</v>
       </c>
-      <c r="F29">
+      <c r="C32">
         <v>0.65399998000000004</v>
       </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A30">
+      <c r="D32" s="1">
+        <v>0.498</v>
+      </c>
+      <c r="E32">
+        <v>0.44800001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
         <v>28</v>
       </c>
-      <c r="E30">
+      <c r="B33">
         <v>0.58300000399999996</v>
       </c>
-      <c r="F30">
+      <c r="C33">
         <v>0.54699998999999999</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A31">
+      <c r="D33" s="1">
+        <v>0.51</v>
+      </c>
+      <c r="E33">
+        <v>0.45800000000000002</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34">
         <v>29</v>
       </c>
-      <c r="E31">
+      <c r="B34">
         <v>0.59399998200000004</v>
       </c>
-      <c r="F31">
+      <c r="C34">
         <v>0.65799998999999998</v>
+      </c>
+      <c r="D34" s="1">
+        <v>0.53400000000000003</v>
+      </c>
+      <c r="E34">
+        <v>0.47099998999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>